<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@128e765e86a3e353cc116e5fbcc3180acd07af58 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-ct-mrt-abdomen.xlsx
+++ b/StructureDefinition-ct-mrt-abdomen.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$56</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="474">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-31T11:09:58+00:00</t>
+    <t>2024-12-02T15:35:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -995,6 +995,104 @@
     <t>subjectOf.observationEvent[code="annotation"].value</t>
   </si>
   <si>
+    <t>Observation.note.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Observation.note.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Observation.note.author[x]</t>
+  </si>
+  <si>
+    <t>Reference(Practitioner|Patient|RelatedPerson|Organization)
+string</t>
+  </si>
+  <si>
+    <t>Individual responsible for the annotation</t>
+  </si>
+  <si>
+    <t>The individual responsible for making the annotation.</t>
+  </si>
+  <si>
+    <t>Organization is used when there's no need for specific attribution as to who made the comment.</t>
+  </si>
+  <si>
+    <t>Annotation.author[x]</t>
+  </si>
+  <si>
+    <t>Act.participant[typeCode=AUT].role</t>
+  </si>
+  <si>
+    <t>Observation.note.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>When the annotation was made</t>
+  </si>
+  <si>
+    <t>Indicates when this particular annotation was made.</t>
+  </si>
+  <si>
+    <t>Annotation.time</t>
+  </si>
+  <si>
+    <t>Act.effectiveTime</t>
+  </si>
+  <si>
+    <t>Observation.note.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">markdown
+</t>
+  </si>
+  <si>
+    <t>The annotation  - text content (as markdown)</t>
+  </si>
+  <si>
+    <t>The text of the annotation in markdown format.</t>
+  </si>
+  <si>
+    <t>Annotation.text</t>
+  </si>
+  <si>
+    <t>Act.text</t>
+  </si>
+  <si>
     <t>Observation.bodySite</t>
   </si>
   <si>
@@ -1141,29 +1239,7 @@
     <t>Observation.referenceRange.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Observation.referenceRange.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Observation.referenceRange.modifierExtension</t>
@@ -1748,7 +1824,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP51"/>
+  <dimension ref="A1:AP56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1785,7 +1861,7 @@
     <col min="26" max="26" width="61.625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
@@ -4840,10 +4916,10 @@
         <v>80</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>20</v>
@@ -4974,17 +5050,15 @@
         <v>20</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="N27" t="s" s="2">
         <v>315</v>
       </c>
+      <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>20</v>
@@ -5009,31 +5083,31 @@
         <v>20</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="Y27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE27" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF27" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF27" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>80</v>
@@ -5045,44 +5119,44 @@
         <v>20</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>318</v>
+        <v>20</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>319</v>
+        <v>20</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP27" t="s" s="2">
-        <v>321</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>20</v>
@@ -5094,20 +5168,18 @@
         <v>20</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>191</v>
+        <v>138</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="O28" t="s" s="2">
-        <v>326</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>20</v>
       </c>
@@ -5131,43 +5203,43 @@
         <v>20</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>327</v>
+        <v>20</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>328</v>
+        <v>20</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="AD28" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>20</v>
+        <v>322</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>20</v>
@@ -5176,10 +5248,10 @@
         <v>20</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>329</v>
+        <v>20</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>20</v>
@@ -5190,10 +5262,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5213,19 +5285,19 @@
         <v>20</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5275,7 +5347,7 @@
         <v>20</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>80</v>
@@ -5293,27 +5365,27 @@
         <v>20</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>336</v>
+        <v>20</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>337</v>
+        <v>135</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP29" t="s" s="2">
-        <v>339</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5333,20 +5405,18 @@
         <v>20</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>344</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>20</v>
@@ -5395,7 +5465,7 @@
         <v>20</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>80</v>
@@ -5413,27 +5483,27 @@
         <v>20</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>345</v>
+        <v>20</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>346</v>
+        <v>135</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP30" t="s" s="2">
-        <v>348</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5441,35 +5511,31 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>20</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="O31" t="s" s="2">
-        <v>354</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
         <v>20</v>
       </c>
@@ -5517,19 +5583,19 @@
         <v>20</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>355</v>
+        <v>104</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>20</v>
@@ -5538,10 +5604,10 @@
         <v>20</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>356</v>
+        <v>135</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>20</v>
@@ -5552,10 +5618,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5578,15 +5644,17 @@
         <v>20</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>359</v>
+        <v>191</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="N32" s="2"/>
+        <v>345</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>346</v>
+      </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>20</v>
@@ -5611,13 +5679,13 @@
         <v>20</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>20</v>
+        <v>347</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>20</v>
+        <v>348</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>20</v>
@@ -5635,7 +5703,7 @@
         <v>20</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>80</v>
@@ -5647,44 +5715,44 @@
         <v>20</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>20</v>
+        <v>350</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP32" t="s" s="2">
-        <v>20</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>20</v>
@@ -5696,18 +5764,20 @@
         <v>20</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>138</v>
+        <v>191</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>139</v>
+        <v>354</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O33" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>357</v>
+      </c>
       <c r="P33" t="s" s="2">
         <v>20</v>
       </c>
@@ -5731,13 +5801,13 @@
         <v>20</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>20</v>
+        <v>359</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>20</v>
@@ -5755,19 +5825,19 @@
         <v>20</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>20</v>
@@ -5776,10 +5846,10 @@
         <v>20</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>20</v>
+        <v>360</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>20</v>
@@ -5790,46 +5860,44 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>368</v>
+        <v>20</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>138</v>
+        <v>363</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O34" t="s" s="2">
-        <v>147</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>20</v>
       </c>
@@ -5877,45 +5945,45 @@
         <v>20</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>20</v>
+        <v>367</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>20</v>
+        <v>368</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>135</v>
+        <v>369</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP34" t="s" s="2">
-        <v>20</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5938,15 +6006,17 @@
         <v>20</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>374</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>375</v>
       </c>
-      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>20</v>
@@ -5995,7 +6065,7 @@
         <v>20</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>80</v>
@@ -6004,7 +6074,7 @@
         <v>92</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>376</v>
+        <v>20</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>104</v>
@@ -6013,7 +6083,7 @@
         <v>20</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>20</v>
+        <v>376</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>377</v>
@@ -6025,15 +6095,15 @@
         <v>20</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>20</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6044,7 +6114,7 @@
         <v>80</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>20</v>
@@ -6056,16 +6126,20 @@
         <v>20</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
+        <v>383</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>385</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>20</v>
       </c>
@@ -6113,19 +6187,19 @@
         <v>20</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>376</v>
+        <v>20</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>104</v>
+        <v>386</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>20</v>
@@ -6134,10 +6208,10 @@
         <v>20</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>20</v>
@@ -6148,10 +6222,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6174,20 +6248,16 @@
         <v>20</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>384</v>
+        <v>314</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>387</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>20</v>
       </c>
@@ -6211,13 +6281,13 @@
         <v>20</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>388</v>
+        <v>20</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>389</v>
+        <v>20</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>20</v>
@@ -6235,7 +6305,7 @@
         <v>20</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>383</v>
+        <v>316</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>80</v>
@@ -6247,19 +6317,19 @@
         <v>20</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>391</v>
+        <v>20</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>20</v>
@@ -6270,14 +6340,14 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
@@ -6296,20 +6366,18 @@
         <v>20</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>191</v>
+        <v>138</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>393</v>
+        <v>139</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>394</v>
+        <v>319</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>396</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>20</v>
       </c>
@@ -6333,13 +6401,13 @@
         <v>20</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>397</v>
+        <v>20</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>398</v>
+        <v>20</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>20</v>
@@ -6357,7 +6425,7 @@
         <v>20</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>392</v>
+        <v>323</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>80</v>
@@ -6369,19 +6437,19 @@
         <v>20</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>391</v>
+        <v>20</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>20</v>
@@ -6392,43 +6460,45 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>20</v>
+        <v>392</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>20</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>400</v>
+        <v>138</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>402</v>
-      </c>
-      <c r="N39" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="O39" t="s" s="2">
-        <v>403</v>
+        <v>147</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>20</v>
@@ -6477,19 +6547,19 @@
         <v>20</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>20</v>
@@ -6501,7 +6571,7 @@
         <v>20</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>404</v>
+        <v>135</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>20</v>
@@ -6512,10 +6582,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6538,13 +6608,13 @@
         <v>20</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>359</v>
+        <v>397</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6595,7 +6665,7 @@
         <v>20</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>80</v>
@@ -6604,7 +6674,7 @@
         <v>92</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>104</v>
@@ -6616,10 +6686,10 @@
         <v>20</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>377</v>
+        <v>401</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>20</v>
@@ -6630,10 +6700,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6644,7 +6714,7 @@
         <v>80</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>20</v>
@@ -6653,20 +6723,18 @@
         <v>20</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>413</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
         <v>20</v>
@@ -6715,16 +6783,16 @@
         <v>20</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>104</v>
@@ -6736,10 +6804,10 @@
         <v>20</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>20</v>
@@ -6750,10 +6818,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6764,7 +6832,7 @@
         <v>80</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>20</v>
@@ -6773,21 +6841,23 @@
         <v>20</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>417</v>
+        <v>191</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="O42" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="O42" t="s" s="2">
+        <v>411</v>
+      </c>
       <c r="P42" t="s" s="2">
         <v>20</v>
       </c>
@@ -6811,13 +6881,13 @@
         <v>20</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>20</v>
+        <v>412</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>20</v>
+        <v>413</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>20</v>
@@ -6835,13 +6905,13 @@
         <v>20</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>20</v>
@@ -6853,13 +6923,13 @@
         <v>20</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>20</v>
+        <v>414</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>421</v>
+        <v>302</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>20</v>
@@ -6870,10 +6940,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6893,22 +6963,22 @@
         <v>20</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>350</v>
+        <v>191</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>20</v>
@@ -6933,13 +7003,13 @@
         <v>20</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>20</v>
+        <v>421</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>20</v>
+        <v>422</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>20</v>
@@ -6957,7 +7027,7 @@
         <v>20</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>80</v>
@@ -6975,13 +7045,13 @@
         <v>20</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>20</v>
+        <v>414</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>428</v>
+        <v>302</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>20</v>
@@ -6992,10 +7062,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7018,16 +7088,18 @@
         <v>20</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>359</v>
+        <v>424</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>360</v>
+        <v>425</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>361</v>
+        <v>426</v>
       </c>
       <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>427</v>
+      </c>
       <c r="P44" t="s" s="2">
         <v>20</v>
       </c>
@@ -7075,7 +7147,7 @@
         <v>20</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>362</v>
+        <v>423</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>80</v>
@@ -7087,7 +7159,7 @@
         <v>20</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>20</v>
@@ -7099,7 +7171,7 @@
         <v>20</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>363</v>
+        <v>428</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>20</v>
@@ -7110,21 +7182,21 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>20</v>
@@ -7136,17 +7208,15 @@
         <v>20</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>138</v>
+        <v>313</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>139</v>
+        <v>430</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>20</v>
@@ -7195,19 +7265,19 @@
         <v>20</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>366</v>
+        <v>429</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>20</v>
@@ -7216,10 +7286,10 @@
         <v>20</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>20</v>
+        <v>401</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>20</v>
@@ -7230,14 +7300,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>368</v>
+        <v>20</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7250,26 +7320,24 @@
         <v>20</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="J46" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>138</v>
+        <v>434</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>369</v>
+        <v>435</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>370</v>
+        <v>436</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O46" t="s" s="2">
-        <v>147</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>20</v>
       </c>
@@ -7317,7 +7385,7 @@
         <v>20</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>371</v>
+        <v>433</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>80</v>
@@ -7329,7 +7397,7 @@
         <v>20</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>20</v>
@@ -7338,10 +7406,10 @@
         <v>20</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>20</v>
+        <v>438</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>135</v>
+        <v>439</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>20</v>
@@ -7352,10 +7420,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7363,10 +7431,10 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>20</v>
@@ -7378,20 +7446,18 @@
         <v>93</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>191</v>
+        <v>441</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>435</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>205</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>20</v>
       </c>
@@ -7415,13 +7481,13 @@
         <v>20</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>208</v>
+        <v>20</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>20</v>
@@ -7439,13 +7505,13 @@
         <v>20</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>20</v>
@@ -7457,16 +7523,16 @@
         <v>20</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>436</v>
+        <v>20</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>212</v>
+        <v>438</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>213</v>
+        <v>445</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>214</v>
+        <v>20</v>
       </c>
       <c r="AP47" t="s" s="2">
         <v>20</v>
@@ -7474,10 +7540,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7488,7 +7554,7 @@
         <v>80</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>20</v>
@@ -7500,19 +7566,19 @@
         <v>93</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>438</v>
+        <v>381</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>273</v>
+        <v>448</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>275</v>
+        <v>450</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>20</v>
@@ -7561,13 +7627,13 @@
         <v>20</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>20</v>
@@ -7579,27 +7645,27 @@
         <v>20</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>441</v>
+        <v>20</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>279</v>
+        <v>451</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>280</v>
+        <v>452</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>281</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7622,20 +7688,16 @@
         <v>20</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>443</v>
+        <v>314</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>286</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
         <v>20</v>
       </c>
@@ -7659,13 +7721,13 @@
         <v>20</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>287</v>
+        <v>20</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>288</v>
+        <v>20</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>289</v>
+        <v>20</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>20</v>
@@ -7683,7 +7745,7 @@
         <v>20</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>442</v>
+        <v>316</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>80</v>
@@ -7692,10 +7754,10 @@
         <v>92</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>290</v>
+        <v>20</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>20</v>
@@ -7704,10 +7766,10 @@
         <v>20</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>20</v>
@@ -7718,14 +7780,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>293</v>
+        <v>137</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7744,20 +7806,18 @@
         <v>20</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>191</v>
+        <v>138</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>294</v>
+        <v>139</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="O50" t="s" s="2">
-        <v>297</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>20</v>
       </c>
@@ -7781,13 +7841,13 @@
         <v>20</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>287</v>
+        <v>20</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>298</v>
+        <v>20</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>299</v>
+        <v>20</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>20</v>
@@ -7805,7 +7865,7 @@
         <v>20</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>446</v>
+        <v>323</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>80</v>
@@ -7817,37 +7877,37 @@
         <v>20</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>301</v>
+        <v>20</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AP50" t="s" s="2">
-        <v>303</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>20</v>
+        <v>392</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
@@ -7860,25 +7920,25 @@
         <v>20</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>448</v>
+        <v>393</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>449</v>
+        <v>394</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>353</v>
+        <v>141</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>354</v>
+        <v>147</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>20</v>
@@ -7927,7 +7987,7 @@
         <v>20</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>447</v>
+        <v>395</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>80</v>
@@ -7939,29 +7999,639 @@
         <v>20</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AO51" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AP51" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="P52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="AK51" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AP51" t="s" s="2">
+      <c r="AK52" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="AP52" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="P53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AP53" t="s" s="2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="P54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AO54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AP54" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="P55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q55" s="2"/>
+      <c r="R55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="AO55" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AP55" t="s" s="2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="P56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AO56" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="AP56" t="s" s="2">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP51">
+  <autoFilter ref="A1:AP56">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7971,7 +8641,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI50">
+  <conditionalFormatting sqref="A2:AI55">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>